<commit_message>
prepare IS for TR
</commit_message>
<xml_diff>
--- a/SSR/update_SSR.xlsx
+++ b/SSR/update_SSR.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ava\Code\DomainModelExtractor\SSR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bo/Documents/projects/DomainModelExtractor/SSR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{565C9720-02B6-45C5-968C-3B7DAD6CE243}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA0BD7E6-122C-0445-8E3E-CD84DCAFCE3E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1008" yWindow="-108" windowWidth="22140" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1000" yWindow="460" windowWidth="22140" windowHeight="13180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="update_SSR" sheetId="1" r:id="rId1"/>
@@ -35,9 +35,6 @@
     <t>POS-tags</t>
   </si>
   <si>
-    <t>start word</t>
-  </si>
-  <si>
     <t>sentence example</t>
   </si>
   <si>
@@ -887,13 +884,16 @@
   </si>
   <si>
     <t>prep,pobj</t>
+  </si>
+  <si>
+    <t>Keywords</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1772,17 +1772,17 @@
   <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="20.33203125" customWidth="1"/>
     <col min="3" max="3" width="55.6640625" customWidth="1"/>
     <col min="5" max="5" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1796,489 +1796,489 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>163</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" t="s">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>126</v>
+      </c>
+      <c r="F3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
         <v>127</v>
       </c>
-      <c r="F3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="F4" t="s">
         <v>14</v>
       </c>
-      <c r="C4" t="s">
-        <v>128</v>
-      </c>
-      <c r="F4" t="s">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
         <v>16</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
+        <v>134</v>
+      </c>
+      <c r="F5" t="s">
         <v>17</v>
       </c>
-      <c r="C5" t="s">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>130</v>
+      </c>
+      <c r="F6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
         <v>135</v>
       </c>
-      <c r="F5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" t="s">
-        <v>131</v>
-      </c>
-      <c r="F6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="F7" t="s">
         <v>23</v>
       </c>
-      <c r="C7" t="s">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
         <v>136</v>
       </c>
-      <c r="F7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="F8" t="s">
         <v>26</v>
       </c>
-      <c r="C8" t="s">
-        <v>137</v>
-      </c>
-      <c r="F8" t="s">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" t="s">
+      <c r="B9" t="s">
         <v>28</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
+        <v>138</v>
+      </c>
+      <c r="D9" t="s">
         <v>29</v>
       </c>
-      <c r="C9" t="s">
-        <v>139</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="F9" t="s">
         <v>30</v>
       </c>
-      <c r="F9" t="s">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" t="s">
+      <c r="B10" t="s">
         <v>32</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
+        <v>138</v>
+      </c>
+      <c r="D10" t="s">
         <v>33</v>
       </c>
-      <c r="C10" t="s">
-        <v>139</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="F10" t="s">
         <v>34</v>
       </c>
-      <c r="F10" t="s">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" t="s">
+      <c r="B11" t="s">
         <v>36</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>37</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>38</v>
       </c>
-      <c r="D11" t="s">
+      <c r="F11" t="s">
         <v>39</v>
       </c>
-      <c r="F11" t="s">
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" t="s">
+      <c r="B12" t="s">
         <v>41</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" t="s">
         <v>42</v>
       </c>
-      <c r="C12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="F12" t="s">
         <v>43</v>
       </c>
-      <c r="F12" t="s">
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" t="s">
+      <c r="B13" t="s">
         <v>45</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F13" t="s">
         <v>46</v>
       </c>
-      <c r="C13" t="s">
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" t="s">
         <v>153</v>
       </c>
-      <c r="F13" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="F14" t="s">
         <v>49</v>
       </c>
-      <c r="C14" t="s">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" t="s">
         <v>154</v>
       </c>
-      <c r="F14" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" t="s">
-        <v>51</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="F15" t="s">
         <v>52</v>
       </c>
-      <c r="C15" t="s">
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" t="s">
+        <v>55</v>
+      </c>
+      <c r="F16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" t="s">
+        <v>96</v>
+      </c>
+      <c r="F17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" t="s">
         <v>155</v>
       </c>
-      <c r="F15" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" t="s">
-        <v>54</v>
-      </c>
-      <c r="B16" t="s">
-        <v>55</v>
-      </c>
-      <c r="C16" t="s">
-        <v>56</v>
-      </c>
-      <c r="F16" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" t="s">
-        <v>58</v>
-      </c>
-      <c r="B17" t="s">
-        <v>59</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="F18" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" t="s">
+        <v>64</v>
+      </c>
+      <c r="C19" t="s">
+        <v>65</v>
+      </c>
+      <c r="F19" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20" t="s">
+        <v>145</v>
+      </c>
+      <c r="F20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>70</v>
+      </c>
+      <c r="B21" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" t="s">
+        <v>72</v>
+      </c>
+      <c r="F21" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>74</v>
+      </c>
+      <c r="B22" t="s">
+        <v>75</v>
+      </c>
+      <c r="C22" t="s">
+        <v>76</v>
+      </c>
+      <c r="F22" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>78</v>
+      </c>
+      <c r="B23" t="s">
+        <v>79</v>
+      </c>
+      <c r="C23" t="s">
+        <v>80</v>
+      </c>
+      <c r="F23" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>82</v>
+      </c>
+      <c r="B24" t="s">
+        <v>83</v>
+      </c>
+      <c r="C24" t="s">
+        <v>158</v>
+      </c>
+      <c r="F24" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>85</v>
+      </c>
+      <c r="B25" t="s">
+        <v>86</v>
+      </c>
+      <c r="C25" t="s">
+        <v>159</v>
+      </c>
+      <c r="F25" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>88</v>
+      </c>
+      <c r="B26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C26" t="s">
+        <v>160</v>
+      </c>
+      <c r="F26" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>91</v>
+      </c>
+      <c r="B27" t="s">
+        <v>92</v>
+      </c>
+      <c r="C27" t="s">
+        <v>161</v>
+      </c>
+      <c r="F27" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>94</v>
+      </c>
+      <c r="B28" t="s">
+        <v>95</v>
+      </c>
+      <c r="C28" t="s">
+        <v>96</v>
+      </c>
+      <c r="F28" t="s">
         <v>97</v>
       </c>
-      <c r="F17" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" t="s">
-        <v>61</v>
-      </c>
-      <c r="B18" t="s">
-        <v>62</v>
-      </c>
-      <c r="C18" t="s">
-        <v>156</v>
-      </c>
-      <c r="F18" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" t="s">
-        <v>64</v>
-      </c>
-      <c r="B19" t="s">
-        <v>65</v>
-      </c>
-      <c r="C19" t="s">
-        <v>66</v>
-      </c>
-      <c r="F19" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" t="s">
-        <v>68</v>
-      </c>
-      <c r="B20" t="s">
-        <v>69</v>
-      </c>
-      <c r="C20" t="s">
-        <v>146</v>
-      </c>
-      <c r="F20" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" t="s">
-        <v>71</v>
-      </c>
-      <c r="B21" t="s">
-        <v>72</v>
-      </c>
-      <c r="C21" t="s">
-        <v>73</v>
-      </c>
-      <c r="F21" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" t="s">
-        <v>75</v>
-      </c>
-      <c r="B22" t="s">
-        <v>76</v>
-      </c>
-      <c r="C22" t="s">
-        <v>77</v>
-      </c>
-      <c r="F22" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" t="s">
-        <v>79</v>
-      </c>
-      <c r="B23" t="s">
-        <v>80</v>
-      </c>
-      <c r="C23" t="s">
-        <v>81</v>
-      </c>
-      <c r="F23" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" t="s">
-        <v>83</v>
-      </c>
-      <c r="B24" t="s">
-        <v>84</v>
-      </c>
-      <c r="C24" t="s">
-        <v>159</v>
-      </c>
-      <c r="F24" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" t="s">
-        <v>86</v>
-      </c>
-      <c r="B25" t="s">
-        <v>87</v>
-      </c>
-      <c r="C25" t="s">
-        <v>160</v>
-      </c>
-      <c r="F25" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" t="s">
-        <v>89</v>
-      </c>
-      <c r="B26" t="s">
-        <v>90</v>
-      </c>
-      <c r="C26" t="s">
-        <v>161</v>
-      </c>
-      <c r="F26" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" t="s">
-        <v>92</v>
-      </c>
-      <c r="B27" t="s">
-        <v>93</v>
-      </c>
-      <c r="C27" t="s">
-        <v>162</v>
-      </c>
-      <c r="F27" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" t="s">
-        <v>95</v>
-      </c>
-      <c r="B28" t="s">
-        <v>96</v>
-      </c>
-      <c r="C28" t="s">
-        <v>97</v>
-      </c>
-      <c r="F28" t="s">
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" t="s">
+      <c r="B29" t="s">
         <v>99</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>100</v>
       </c>
-      <c r="C29" t="s">
+      <c r="F29" t="s">
         <v>101</v>
       </c>
-      <c r="F29" t="s">
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" t="s">
+      <c r="B30" t="s">
         <v>103</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>104</v>
       </c>
-      <c r="C30" t="s">
+      <c r="F30" t="s">
         <v>105</v>
       </c>
-      <c r="F30" t="s">
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" t="s">
+      <c r="B31" t="s">
         <v>107</v>
       </c>
-      <c r="B31" t="s">
+      <c r="E31" t="s">
         <v>108</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
         <v>109</v>
       </c>
-      <c r="F31" t="s">
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" t="s">
+      <c r="B32" t="s">
         <v>111</v>
       </c>
-      <c r="B32" t="s">
+      <c r="E32" t="s">
         <v>112</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32" t="s">
         <v>113</v>
       </c>
-      <c r="F32" t="s">
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="A33" t="s">
+      <c r="B33" t="s">
         <v>115</v>
       </c>
-      <c r="B33" t="s">
+      <c r="E33" t="s">
         <v>116</v>
       </c>
-      <c r="E33" t="s">
+      <c r="F33" t="s">
         <v>117</v>
       </c>
-      <c r="F33" t="s">
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34" t="s">
+      <c r="B34" t="s">
         <v>119</v>
       </c>
-      <c r="B34" t="s">
+      <c r="E34" t="s">
         <v>120</v>
       </c>
-      <c r="E34" t="s">
+      <c r="F34" t="s">
         <v>121</v>
       </c>
-      <c r="F34" t="s">
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>122</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" t="s">
-        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -2295,419 +2295,419 @@
       <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="8.88671875" style="1"/>
-    <col min="3" max="3" width="14.88671875" style="1" customWidth="1"/>
-    <col min="4" max="5" width="8.88671875" style="1"/>
+    <col min="1" max="2" width="8.83203125" style="1"/>
+    <col min="3" max="3" width="14.83203125" style="1" customWidth="1"/>
+    <col min="4" max="5" width="8.83203125" style="1"/>
     <col min="6" max="6" width="14.6640625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="1"/>
+    <col min="7" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="I2" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="I1" s="1" t="s">
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="I5" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="L24" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
-      <c r="A2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="I2" s="1" t="s">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="3" spans="1:12">
-      <c r="A3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
-      <c r="A4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="A5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="I5" s="1" t="s">
+      <c r="E25" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
-      <c r="A7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="I7" s="1" t="s">
+      <c r="I28" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="A8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="A9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="A10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="I10" s="1" t="s">
+      <c r="I29" s="1" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
-      <c r="A11" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
-      <c r="A12" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
-      <c r="A13" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12">
-      <c r="A14" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12">
-      <c r="A15" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12">
-      <c r="A16" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12">
-      <c r="A17" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="L17" s="1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12">
-      <c r="A18" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12">
-      <c r="A19" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12">
-      <c r="A20" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12">
-      <c r="A21" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12">
-      <c r="A22" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12">
-      <c r="A23" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12">
-      <c r="A24" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="L24" s="1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12">
-      <c r="A25" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="L25" s="1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12">
-      <c r="A26" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="L26" s="1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12">
-      <c r="A27" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="L27" s="1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12">
-      <c r="A28" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12">
-      <c r="A29" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>